<commit_message>
feat(fpu): add support for 32 bit addition #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fputestingprogrambasicoperations.xlsx
+++ b/programs/pipelining/fputestingprogrambasicoperations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0502E9D3-2DCD-4909-9F20-EF6F2677B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F29DCE-F8E2-47AD-B15F-C1E9679175BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2186,15 +2184,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="A7:S7"/>
     <mergeCell ref="A24:S24"/>
     <mergeCell ref="G4:H4"/>
@@ -2207,6 +2196,15 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="K6:P6"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2219,7 +2217,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2732,12 +2730,11 @@
       <c r="Z19" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:Z1"/>
-    <mergeCell ref="D19:Z19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(fpu): fix 16 bit subtraction #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fputestingprogrambasicoperations.xlsx
+++ b/programs/pipelining/fputestingprogrambasicoperations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F29DCE-F8E2-47AD-B15F-C1E9679175BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A077A6-1191-4FD5-B552-99D597B93EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>A - B = 1 in IEEE754</t>
   </si>
   <si>
-    <t>B - A = -1 in IEE754</t>
-  </si>
-  <si>
     <t>A * B = 42 in IEEE754</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>FMUL R3, R2</t>
+  </si>
+  <si>
+    <t>B - A = -1 in IEEE754</t>
   </si>
 </sst>
 </file>
@@ -303,10 +303,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,18 +621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C1">
         <v>15</v>
       </c>
@@ -682,79 +682,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5" t="s">
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -770,10 +770,10 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
@@ -786,99 +786,99 @@
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5" t="s">
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -899,12 +899,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -959,12 +959,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>B44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1079,12 +1079,12 @@
         <v>CC01</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>1C02</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1259,12 +1259,12 @@
         <v>CC01</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>1D02</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1439,12 +1439,12 @@
         <v>CC02</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1499,7 +1499,7 @@
         <v>1D01</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1619,12 +1619,12 @@
         <v>CC01</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1679,7 +1679,7 @@
         <v>1E02</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>D44</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1799,30 +1799,30 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>4A80</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2062,12 +2062,12 @@
         <v>3C00</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2118,16 +2118,16 @@
         <v>0</v>
       </c>
       <c r="S29" s="2" t="str">
-        <f t="shared" ref="S29:S30" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
+        <f t="shared" ref="S29:S31" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
         <v>BC00</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2181,6 +2181,9 @@
         <f t="shared" si="2"/>
         <v>5140</v>
       </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="S31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -2216,60 +2219,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71D0FB5-FE2B-4468-A391-3F433659BE14}">
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="2" customWidth="1"/>
-    <col min="4" max="26" width="7.44140625" style="2" customWidth="1"/>
-    <col min="27" max="29" width="5.44140625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.20703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" style="2" customWidth="1"/>
+    <col min="4" max="26" width="7.41796875" style="2" customWidth="1"/>
+    <col min="27" max="29" width="5.41796875" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
       <c r="AC1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2">
         <v>0</v>
       </c>
@@ -2342,7 +2345,7 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2355,17 +2358,17 @@
         <v>600</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2378,19 +2381,19 @@
         <v>B44</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2403,16 +2406,16 @@
         <v>CC01</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2425,16 +2428,16 @@
         <v>1C02</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2447,19 +2450,19 @@
         <v>D44</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2472,17 +2475,17 @@
         <v>CC01</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2495,17 +2498,17 @@
         <v>1D02</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC9"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2518,20 +2521,20 @@
         <v>D44</v>
       </c>
       <c r="M10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2544,18 +2547,18 @@
         <v>CC02</v>
       </c>
       <c r="O11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="AB11"/>
       <c r="AC11"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2568,18 +2571,18 @@
         <v>1D01</v>
       </c>
       <c r="P12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2592,21 +2595,21 @@
         <v>D44</v>
       </c>
       <c r="Q13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="AB13"/>
       <c r="AC13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2619,17 +2622,17 @@
         <v>CC01</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC14"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2642,20 +2645,20 @@
         <v>1E02</v>
       </c>
       <c r="T15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="W15" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC15"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2668,20 +2671,20 @@
         <v>D44</v>
       </c>
       <c r="V16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="W16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="X16" s="2" t="s">
+      <c r="Y16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Y16" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC16"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2694,40 +2697,40 @@
         <v>7000</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Z17" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AC17"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
fix(fpu): fix the half precision multiplication #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fputestingprogrambasicoperations.xlsx
+++ b/programs/pipelining/fputestingprogrambasicoperations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A077A6-1191-4FD5-B552-99D597B93EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD7981E-D56F-4775-AF33-CE177048FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -621,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="C31" sqref="C31:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="2" t="str">
-        <f t="shared" ref="S29:S31" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
+        <f t="shared" ref="S29:S32" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
         <v>BC00</v>
       </c>
     </row>
@@ -2185,8 +2185,20 @@
     <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="S31" s="2"/>
     </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="S32" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="A7:S7"/>
     <mergeCell ref="A24:S24"/>
     <mergeCell ref="G4:H4"/>
@@ -2199,15 +2211,6 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="K6:P6"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(fpu): fix 32 bit FPU multiplication #2
</commit_message>
<xml_diff>
--- a/programs/pipelining/fputestingprogrambasicoperations.xlsx
+++ b/programs/pipelining/fputestingprogrambasicoperations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD7981E-D56F-4775-AF33-CE177048FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4880622A-432C-47D8-9E38-E4C893B2A967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -181,9 +181,6 @@
     <t>MOV R3 = R2 LSL #0</t>
   </si>
   <si>
-    <t>STOP</t>
-  </si>
-  <si>
     <t>A + B = 13 in IEEE754</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>B - A = -1 in IEEE754</t>
+  </si>
+  <si>
+    <t>STP</t>
   </si>
 </sst>
 </file>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:S33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -857,7 +857,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -904,7 +904,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -964,7 +964,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1264,7 +1264,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1444,7 +1444,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1744,7 +1744,7 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1947,7 +1947,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2007,7 +2007,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="2" t="str">
-        <f t="shared" ref="S29:S32" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
+        <f t="shared" ref="S29:S30" si="2">DEC2HEX(C29*2^15 + D29*2^14 + E29*2^13 + F29*2^12 + G29*2^11 + H29*2^10 + I29*2^9 + J29*2^8 + K29*2^7 + L29*2^6 + M29*2^5 + N29*2^4 + O29 * 2 ^ 3 + P29  * 2^2 + Q29 * 2 + R29)</f>
         <v>BC00</v>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2190,15 +2190,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="A7:S7"/>
     <mergeCell ref="A24:S24"/>
     <mergeCell ref="G4:H4"/>
@@ -2211,6 +2202,15 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="K6:P6"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2237,16 +2237,16 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2361,13 +2361,13 @@
         <v>600</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AD3" s="2"/>
     </row>
@@ -2384,16 +2384,16 @@
         <v>B44</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
@@ -2409,13 +2409,13 @@
         <v>CC01</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
@@ -2431,13 +2431,13 @@
         <v>1C02</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
@@ -2453,16 +2453,16 @@
         <v>D44</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
@@ -2478,13 +2478,13 @@
         <v>CC01</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC8"/>
     </row>
@@ -2501,13 +2501,13 @@
         <v>1D02</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC9"/>
     </row>
@@ -2524,16 +2524,16 @@
         <v>D44</v>
       </c>
       <c r="M10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC10"/>
     </row>
@@ -2550,13 +2550,13 @@
         <v>CC02</v>
       </c>
       <c r="O11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AB11"/>
       <c r="AC11"/>
@@ -2574,13 +2574,13 @@
         <v>1D01</v>
       </c>
       <c r="P12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -2598,16 +2598,16 @@
         <v>D44</v>
       </c>
       <c r="Q13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AB13"/>
       <c r="AC13"/>
@@ -2625,13 +2625,13 @@
         <v>CC01</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC14"/>
     </row>
@@ -2648,16 +2648,16 @@
         <v>1E02</v>
       </c>
       <c r="T15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC15"/>
     </row>
@@ -2674,16 +2674,16 @@
         <v>D44</v>
       </c>
       <c r="V16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X16" s="2" t="s">
+      <c r="Y16" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC16"/>
     </row>
@@ -2693,20 +2693,20 @@
       </c>
       <c r="B17" t="str">
         <f>Code!B23</f>
-        <v>STOP</v>
+        <v>STP</v>
       </c>
       <c r="C17" s="2" t="str">
         <f>Code!S23</f>
         <v>7000</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="Z17" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AC17"/>
     </row>

</xml_diff>